<commit_message>
echelle 2 brightness conversion
</commit_message>
<xml_diff>
--- a/data_processing/2024/OES/data/echelle_db.xlsx
+++ b/data_processing/2024/OES/data/echelle_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickmartinez/Library/Mobile Documents/com~apple~CloudDocs/Documents/GitHub/relozwall/data_processing/2024/OES/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8C1809-B458-BA49-A651-AC6CA5C1F488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1949D099-63DC-1542-BEBC-F5DC527878CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,27 @@
     <sheet name="Spectrometer parameters" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Spectrometer parameters'!$A$1:$P$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Spectrometer parameters'!$A$1:$Q$73</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="63">
   <si>
     <t>Folder</t>
   </si>
@@ -194,6 +207,24 @@
   </si>
   <si>
     <t>Is dark</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Boron rod</t>
+  </si>
+  <si>
+    <t>Boron pebble rod</t>
+  </si>
+  <si>
+    <t>Labsphere</t>
+  </si>
+  <si>
+    <t>echelle_20241003</t>
+  </si>
+  <si>
+    <t>Poly boron pebble rod</t>
   </si>
 </sst>
 </file>
@@ -215,6 +246,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -266,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -279,6 +311,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,11 +618,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P73"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -599,7 +635,7 @@
     <col min="15" max="15" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -648,8 +684,11 @@
       <c r="P1" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -698,8 +737,11 @@
       <c r="P2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -748,8 +790,11 @@
       <c r="P3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -798,8 +843,11 @@
       <c r="P4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -848,8 +896,11 @@
       <c r="P5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -898,8 +949,11 @@
       <c r="P6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -948,8 +1002,11 @@
       <c r="P7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -998,8 +1055,11 @@
       <c r="P8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1048,8 +1108,11 @@
       <c r="P9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1098,8 +1161,11 @@
       <c r="P10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1148,8 +1214,11 @@
       <c r="P11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1198,8 +1267,11 @@
       <c r="P12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1248,8 +1320,11 @@
       <c r="P13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1298,8 +1373,11 @@
       <c r="P14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1348,8 +1426,11 @@
       <c r="P15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1398,8 +1479,11 @@
       <c r="P16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1448,8 +1532,11 @@
       <c r="P17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1498,8 +1585,11 @@
       <c r="P18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1548,8 +1638,11 @@
       <c r="P19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1598,8 +1691,11 @@
       <c r="P20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1648,8 +1744,11 @@
       <c r="P21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1698,8 +1797,11 @@
       <c r="P22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1748,8 +1850,11 @@
       <c r="P23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1798,8 +1903,11 @@
       <c r="P24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1846,10 +1954,13 @@
         <v>23.6</v>
       </c>
       <c r="P25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1896,10 +2007,13 @@
         <v>23.7</v>
       </c>
       <c r="P26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1948,8 +2062,11 @@
       <c r="P27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1998,8 +2115,11 @@
       <c r="P28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2048,8 +2168,11 @@
       <c r="P29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2098,8 +2221,11 @@
       <c r="P30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -2148,8 +2274,11 @@
       <c r="P31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2198,8 +2327,11 @@
       <c r="P32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -2248,8 +2380,11 @@
       <c r="P33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -2298,8 +2433,11 @@
       <c r="P34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2348,8 +2486,11 @@
       <c r="P35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2398,8 +2539,11 @@
       <c r="P36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -2448,8 +2592,11 @@
       <c r="P37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2498,8 +2645,11 @@
       <c r="P38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -2548,8 +2698,11 @@
       <c r="P39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -2598,8 +2751,11 @@
       <c r="P40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2648,8 +2804,11 @@
       <c r="P41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2698,8 +2857,11 @@
       <c r="P42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -2748,8 +2910,11 @@
       <c r="P43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2798,8 +2963,11 @@
       <c r="P44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2848,8 +3016,11 @@
       <c r="P45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2898,8 +3069,11 @@
       <c r="P46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2948,8 +3122,11 @@
       <c r="P47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -2998,8 +3175,11 @@
       <c r="P48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -3048,8 +3228,11 @@
       <c r="P49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -3098,8 +3281,11 @@
       <c r="P50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -3148,8 +3334,11 @@
       <c r="P51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>44</v>
       </c>
@@ -3198,8 +3387,11 @@
       <c r="P52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>44</v>
       </c>
@@ -3248,8 +3440,11 @@
       <c r="P53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>44</v>
       </c>
@@ -3298,8 +3493,11 @@
       <c r="P54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -3348,8 +3546,11 @@
       <c r="P55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -3398,8 +3599,11 @@
       <c r="P56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>44</v>
       </c>
@@ -3448,8 +3652,11 @@
       <c r="P57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>44</v>
       </c>
@@ -3498,8 +3705,11 @@
       <c r="P58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>44</v>
       </c>
@@ -3548,8 +3758,11 @@
       <c r="P59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>44</v>
       </c>
@@ -3596,10 +3809,13 @@
         <v>23.3</v>
       </c>
       <c r="P60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>44</v>
       </c>
@@ -3646,10 +3862,13 @@
         <v>23.3</v>
       </c>
       <c r="P61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>55</v>
       </c>
@@ -3698,8 +3917,11 @@
       <c r="P62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -3748,8 +3970,11 @@
       <c r="P63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -3798,8 +4023,11 @@
       <c r="P64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>55</v>
       </c>
@@ -3848,8 +4076,11 @@
       <c r="P65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>55</v>
       </c>
@@ -3898,8 +4129,11 @@
       <c r="P66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -3948,8 +4182,11 @@
       <c r="P67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -3998,8 +4235,11 @@
       <c r="P68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>55</v>
       </c>
@@ -4048,8 +4288,11 @@
       <c r="P69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q69" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>55</v>
       </c>
@@ -4098,8 +4341,11 @@
       <c r="P70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q70" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -4148,8 +4394,11 @@
       <c r="P71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q71" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -4198,8 +4447,11 @@
       <c r="P72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q72" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -4248,9 +4500,1503 @@
       <c r="P73">
         <v>1</v>
       </c>
+      <c r="Q73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="1">
+        <v>45568.401331018518</v>
+      </c>
+      <c r="D74" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74">
+        <v>0.2</v>
+      </c>
+      <c r="G74">
+        <v>20</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>6.5</v>
+      </c>
+      <c r="J74">
+        <v>3</v>
+      </c>
+      <c r="K74">
+        <v>4</v>
+      </c>
+      <c r="L74">
+        <v>3000</v>
+      </c>
+      <c r="M74">
+        <v>200000000</v>
+      </c>
+      <c r="N74">
+        <v>130</v>
+      </c>
+      <c r="O74">
+        <v>21.5</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="1">
+        <v>45568.401817129627</v>
+      </c>
+      <c r="D75" t="s">
+        <v>17</v>
+      </c>
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75">
+        <v>0.1</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>6.5</v>
+      </c>
+      <c r="J75">
+        <v>3</v>
+      </c>
+      <c r="K75">
+        <v>4</v>
+      </c>
+      <c r="L75">
+        <v>3000</v>
+      </c>
+      <c r="M75">
+        <v>100000000</v>
+      </c>
+      <c r="N75">
+        <v>130</v>
+      </c>
+      <c r="O75">
+        <v>21.5</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" s="1">
+        <v>45568.401944444442</v>
+      </c>
+      <c r="D76" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76">
+        <v>0.1</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>6.5</v>
+      </c>
+      <c r="J76">
+        <v>3</v>
+      </c>
+      <c r="K76">
+        <v>4</v>
+      </c>
+      <c r="L76">
+        <v>3000</v>
+      </c>
+      <c r="M76">
+        <v>100000000</v>
+      </c>
+      <c r="N76">
+        <v>130</v>
+      </c>
+      <c r="O76">
+        <v>21.5</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" s="1">
+        <v>45568.402372685188</v>
+      </c>
+      <c r="D77" t="s">
+        <v>17</v>
+      </c>
+      <c r="E77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77">
+        <v>0.1</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>6.5</v>
+      </c>
+      <c r="J77">
+        <v>3</v>
+      </c>
+      <c r="K77">
+        <v>4</v>
+      </c>
+      <c r="L77">
+        <v>3000</v>
+      </c>
+      <c r="M77">
+        <v>50000000</v>
+      </c>
+      <c r="N77">
+        <v>130</v>
+      </c>
+      <c r="O77">
+        <v>21.5</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" s="1">
+        <v>45568.403692129628</v>
+      </c>
+      <c r="D78" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78">
+        <v>0.1</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>6.5</v>
+      </c>
+      <c r="J78">
+        <v>3</v>
+      </c>
+      <c r="K78">
+        <v>4</v>
+      </c>
+      <c r="L78">
+        <v>3000</v>
+      </c>
+      <c r="M78">
+        <v>50000000</v>
+      </c>
+      <c r="N78">
+        <v>130</v>
+      </c>
+      <c r="O78">
+        <v>21.5</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="1">
+        <v>45568.404305555552</v>
+      </c>
+      <c r="D79" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>20</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>6.5</v>
+      </c>
+      <c r="J79">
+        <v>3</v>
+      </c>
+      <c r="K79">
+        <v>4</v>
+      </c>
+      <c r="L79">
+        <v>3000</v>
+      </c>
+      <c r="M79">
+        <v>1000000000</v>
+      </c>
+      <c r="N79">
+        <v>130</v>
+      </c>
+      <c r="O79">
+        <v>21.6</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>61</v>
+      </c>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="1">
+        <v>45568.406238425923</v>
+      </c>
+      <c r="D80" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80">
+        <v>0.05</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>6.5</v>
+      </c>
+      <c r="J80">
+        <v>3</v>
+      </c>
+      <c r="K80">
+        <v>4</v>
+      </c>
+      <c r="L80">
+        <v>3000</v>
+      </c>
+      <c r="M80">
+        <v>50000000</v>
+      </c>
+      <c r="N80">
+        <v>130</v>
+      </c>
+      <c r="O80">
+        <v>21.6</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>61</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="1">
+        <v>45568.406608796293</v>
+      </c>
+      <c r="D81" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="G81">
+        <v>20</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>6.5</v>
+      </c>
+      <c r="J81">
+        <v>3</v>
+      </c>
+      <c r="K81">
+        <v>4</v>
+      </c>
+      <c r="L81">
+        <v>3000</v>
+      </c>
+      <c r="M81">
+        <v>1000000000</v>
+      </c>
+      <c r="N81">
+        <v>130</v>
+      </c>
+      <c r="O81">
+        <v>21.6</v>
+      </c>
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>61</v>
+      </c>
+      <c r="B82" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="1">
+        <v>45568.409629629627</v>
+      </c>
+      <c r="D82" t="s">
+        <v>17</v>
+      </c>
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>6.5</v>
+      </c>
+      <c r="J82">
+        <v>3</v>
+      </c>
+      <c r="K82">
+        <v>4</v>
+      </c>
+      <c r="L82">
+        <v>3000</v>
+      </c>
+      <c r="M82">
+        <v>1000000000</v>
+      </c>
+      <c r="N82">
+        <v>130</v>
+      </c>
+      <c r="O82">
+        <v>21.7</v>
+      </c>
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>61</v>
+      </c>
+      <c r="B83" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="1">
+        <v>45568.410439814812</v>
+      </c>
+      <c r="D83" t="s">
+        <v>17</v>
+      </c>
+      <c r="E83" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83">
+        <v>0.05</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>6.5</v>
+      </c>
+      <c r="J83">
+        <v>3</v>
+      </c>
+      <c r="K83">
+        <v>4</v>
+      </c>
+      <c r="L83">
+        <v>3000</v>
+      </c>
+      <c r="M83">
+        <v>50000000</v>
+      </c>
+      <c r="N83">
+        <v>130</v>
+      </c>
+      <c r="O83">
+        <v>21.7</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="1">
+        <v>45568.413576388892</v>
+      </c>
+      <c r="D84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84">
+        <v>0.05</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>6.5</v>
+      </c>
+      <c r="J84">
+        <v>3</v>
+      </c>
+      <c r="K84">
+        <v>4</v>
+      </c>
+      <c r="L84">
+        <v>3000</v>
+      </c>
+      <c r="M84">
+        <v>50000000</v>
+      </c>
+      <c r="N84">
+        <v>130</v>
+      </c>
+      <c r="O84">
+        <v>21.8</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>61</v>
+      </c>
+      <c r="B85" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="1">
+        <v>45568.413831018523</v>
+      </c>
+      <c r="D85" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85">
+        <v>20</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>6.5</v>
+      </c>
+      <c r="J85">
+        <v>3</v>
+      </c>
+      <c r="K85">
+        <v>4</v>
+      </c>
+      <c r="L85">
+        <v>3000</v>
+      </c>
+      <c r="M85">
+        <v>1000000000</v>
+      </c>
+      <c r="N85">
+        <v>130</v>
+      </c>
+      <c r="O85">
+        <v>21.9</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>61</v>
+      </c>
+      <c r="B86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="1">
+        <v>45568.42</v>
+      </c>
+      <c r="D86" t="s">
+        <v>17</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="G86">
+        <v>20</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>6.5</v>
+      </c>
+      <c r="J86">
+        <v>3</v>
+      </c>
+      <c r="K86">
+        <v>4</v>
+      </c>
+      <c r="L86">
+        <v>3000</v>
+      </c>
+      <c r="M86">
+        <v>1000000000</v>
+      </c>
+      <c r="N86">
+        <v>130</v>
+      </c>
+      <c r="O86">
+        <v>22</v>
+      </c>
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>61</v>
+      </c>
+      <c r="B87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C87" s="1">
+        <v>45568.420694444438</v>
+      </c>
+      <c r="D87" t="s">
+        <v>17</v>
+      </c>
+      <c r="E87" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87">
+        <v>0.05</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>6.5</v>
+      </c>
+      <c r="J87">
+        <v>3</v>
+      </c>
+      <c r="K87">
+        <v>4</v>
+      </c>
+      <c r="L87">
+        <v>3000</v>
+      </c>
+      <c r="M87">
+        <v>50000000</v>
+      </c>
+      <c r="N87">
+        <v>130</v>
+      </c>
+      <c r="O87">
+        <v>22</v>
+      </c>
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="1">
+        <v>45568.423032407409</v>
+      </c>
+      <c r="D88" t="s">
+        <v>17</v>
+      </c>
+      <c r="E88" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88">
+        <v>0.05</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>6.5</v>
+      </c>
+      <c r="J88">
+        <v>3</v>
+      </c>
+      <c r="K88">
+        <v>4</v>
+      </c>
+      <c r="L88">
+        <v>3000</v>
+      </c>
+      <c r="M88">
+        <v>50000000</v>
+      </c>
+      <c r="N88">
+        <v>130</v>
+      </c>
+      <c r="O88">
+        <v>22.1</v>
+      </c>
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" s="1">
+        <v>45568.423275462963</v>
+      </c>
+      <c r="D89" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="G89">
+        <v>20</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89">
+        <v>6.5</v>
+      </c>
+      <c r="J89">
+        <v>3</v>
+      </c>
+      <c r="K89">
+        <v>4</v>
+      </c>
+      <c r="L89">
+        <v>3000</v>
+      </c>
+      <c r="M89">
+        <v>1000000000</v>
+      </c>
+      <c r="N89">
+        <v>130</v>
+      </c>
+      <c r="O89">
+        <v>22.1</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>61</v>
+      </c>
+      <c r="B90" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="1">
+        <v>45568.43172453704</v>
+      </c>
+      <c r="D90" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" t="s">
+        <v>20</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>20</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90">
+        <v>6.5</v>
+      </c>
+      <c r="J90">
+        <v>3</v>
+      </c>
+      <c r="K90">
+        <v>4</v>
+      </c>
+      <c r="L90">
+        <v>3000</v>
+      </c>
+      <c r="M90">
+        <v>1000000000</v>
+      </c>
+      <c r="N90">
+        <v>130</v>
+      </c>
+      <c r="O90">
+        <v>22.4</v>
+      </c>
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" t="s">
+        <v>36</v>
+      </c>
+      <c r="C91" s="1">
+        <v>45568.432314814818</v>
+      </c>
+      <c r="D91" t="s">
+        <v>17</v>
+      </c>
+      <c r="E91" t="s">
+        <v>18</v>
+      </c>
+      <c r="F91">
+        <v>0.05</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91">
+        <v>6.5</v>
+      </c>
+      <c r="J91">
+        <v>3</v>
+      </c>
+      <c r="K91">
+        <v>4</v>
+      </c>
+      <c r="L91">
+        <v>3000</v>
+      </c>
+      <c r="M91">
+        <v>50000000</v>
+      </c>
+      <c r="N91">
+        <v>130</v>
+      </c>
+      <c r="O91">
+        <v>22.5</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" s="1">
+        <v>45568.43478009259</v>
+      </c>
+      <c r="D92" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92">
+        <v>0.05</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="I92">
+        <v>6.5</v>
+      </c>
+      <c r="J92">
+        <v>3</v>
+      </c>
+      <c r="K92">
+        <v>4</v>
+      </c>
+      <c r="L92">
+        <v>3000</v>
+      </c>
+      <c r="M92">
+        <v>50000000</v>
+      </c>
+      <c r="N92">
+        <v>130</v>
+      </c>
+      <c r="O92">
+        <v>22.6</v>
+      </c>
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="1">
+        <v>45568.435023148151</v>
+      </c>
+      <c r="D93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>20</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
+      </c>
+      <c r="I93">
+        <v>6.5</v>
+      </c>
+      <c r="J93">
+        <v>3</v>
+      </c>
+      <c r="K93">
+        <v>4</v>
+      </c>
+      <c r="L93">
+        <v>3000</v>
+      </c>
+      <c r="M93">
+        <v>1000000000</v>
+      </c>
+      <c r="N93">
+        <v>130</v>
+      </c>
+      <c r="O93">
+        <v>22.6</v>
+      </c>
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" s="1">
+        <v>45568.44158564815</v>
+      </c>
+      <c r="D94" t="s">
+        <v>17</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>20</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>6.5</v>
+      </c>
+      <c r="J94">
+        <v>3</v>
+      </c>
+      <c r="K94">
+        <v>4</v>
+      </c>
+      <c r="L94">
+        <v>3000</v>
+      </c>
+      <c r="M94">
+        <v>1000000000</v>
+      </c>
+      <c r="N94">
+        <v>130</v>
+      </c>
+      <c r="O94">
+        <v>22.8</v>
+      </c>
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>61</v>
+      </c>
+      <c r="B95" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="1">
+        <v>45568.442175925928</v>
+      </c>
+      <c r="D95" t="s">
+        <v>17</v>
+      </c>
+      <c r="E95" t="s">
+        <v>18</v>
+      </c>
+      <c r="F95">
+        <v>0.05</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="I95">
+        <v>6.5</v>
+      </c>
+      <c r="J95">
+        <v>3</v>
+      </c>
+      <c r="K95">
+        <v>4</v>
+      </c>
+      <c r="L95">
+        <v>3000</v>
+      </c>
+      <c r="M95">
+        <v>50000000</v>
+      </c>
+      <c r="N95">
+        <v>130</v>
+      </c>
+      <c r="O95">
+        <v>22.8</v>
+      </c>
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" s="1">
+        <v>45568.444733796299</v>
+      </c>
+      <c r="D96" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" t="s">
+        <v>18</v>
+      </c>
+      <c r="F96">
+        <v>0.05</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>6.5</v>
+      </c>
+      <c r="J96">
+        <v>3</v>
+      </c>
+      <c r="K96">
+        <v>4</v>
+      </c>
+      <c r="L96">
+        <v>3000</v>
+      </c>
+      <c r="M96">
+        <v>50000000</v>
+      </c>
+      <c r="N96">
+        <v>130</v>
+      </c>
+      <c r="O96">
+        <v>22.9</v>
+      </c>
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>61</v>
+      </c>
+      <c r="B97" t="s">
+        <v>42</v>
+      </c>
+      <c r="C97" s="1">
+        <v>45568.444965277777</v>
+      </c>
+      <c r="D97" t="s">
+        <v>17</v>
+      </c>
+      <c r="E97" t="s">
+        <v>20</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <v>20</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+      <c r="I97">
+        <v>6.5</v>
+      </c>
+      <c r="J97">
+        <v>3</v>
+      </c>
+      <c r="K97">
+        <v>4</v>
+      </c>
+      <c r="L97">
+        <v>3000</v>
+      </c>
+      <c r="M97">
+        <v>1000000000</v>
+      </c>
+      <c r="N97">
+        <v>130</v>
+      </c>
+      <c r="O97">
+        <v>22.9</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" t="s">
+        <v>43</v>
+      </c>
+      <c r="C98" s="1">
+        <v>45568.447164351863</v>
+      </c>
+      <c r="D98" t="s">
+        <v>17</v>
+      </c>
+      <c r="E98" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <v>20</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>6.5</v>
+      </c>
+      <c r="J98">
+        <v>3</v>
+      </c>
+      <c r="K98">
+        <v>4</v>
+      </c>
+      <c r="L98">
+        <v>3000</v>
+      </c>
+      <c r="M98">
+        <v>1000000000</v>
+      </c>
+      <c r="N98">
+        <v>130</v>
+      </c>
+      <c r="O98">
+        <v>23.1</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" t="s">
+        <v>45</v>
+      </c>
+      <c r="C99" s="1">
+        <v>45568.447777777779</v>
+      </c>
+      <c r="D99" t="s">
+        <v>17</v>
+      </c>
+      <c r="E99" t="s">
+        <v>18</v>
+      </c>
+      <c r="F99">
+        <v>0.05</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+      <c r="I99">
+        <v>6.5</v>
+      </c>
+      <c r="J99">
+        <v>3</v>
+      </c>
+      <c r="K99">
+        <v>4</v>
+      </c>
+      <c r="L99">
+        <v>3000</v>
+      </c>
+      <c r="M99">
+        <v>50000000</v>
+      </c>
+      <c r="N99">
+        <v>130</v>
+      </c>
+      <c r="O99">
+        <v>23</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B100" t="s">
+        <v>46</v>
+      </c>
+      <c r="C100" s="1">
+        <v>45568.450844907413</v>
+      </c>
+      <c r="D100" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" t="s">
+        <v>18</v>
+      </c>
+      <c r="F100">
+        <v>0.05</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+      <c r="I100">
+        <v>6.5</v>
+      </c>
+      <c r="J100">
+        <v>3</v>
+      </c>
+      <c r="K100">
+        <v>4</v>
+      </c>
+      <c r="L100">
+        <v>3000</v>
+      </c>
+      <c r="M100">
+        <v>50000000</v>
+      </c>
+      <c r="N100">
+        <v>130</v>
+      </c>
+      <c r="O100">
+        <v>23.2</v>
+      </c>
+      <c r="P100">
+        <v>1</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" t="s">
+        <v>47</v>
+      </c>
+      <c r="C101" s="1">
+        <v>45568.451064814813</v>
+      </c>
+      <c r="D101" t="s">
+        <v>17</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101">
+        <v>20</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="I101">
+        <v>6.5</v>
+      </c>
+      <c r="J101">
+        <v>3</v>
+      </c>
+      <c r="K101">
+        <v>4</v>
+      </c>
+      <c r="L101">
+        <v>3000</v>
+      </c>
+      <c r="M101">
+        <v>1000000000</v>
+      </c>
+      <c r="N101">
+        <v>130</v>
+      </c>
+      <c r="O101">
+        <v>23.2</v>
+      </c>
+      <c r="P101">
+        <v>1</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P73" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q73" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="echelle_20240827"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
picking data points from plot
</commit_message>
<xml_diff>
--- a/data_processing/2024/OES/data/echelle_db.xlsx
+++ b/data_processing/2024/OES/data/echelle_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickmartinez/Library/Mobile Documents/com~apple~CloudDocs/Documents/GitHub/relozwall/data_processing/2024/OES/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B6E5ED-7B2E-EF46-B64E-FA75A2D7DF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88525A8-0FC8-1948-82EE-83B5AED3DF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spectrometer parameters" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="65">
   <si>
     <t>Folder</t>
   </si>
@@ -627,8 +627,8 @@
   <dimension ref="A1:Q132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U117" sqref="U117"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P131" sqref="P131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7632,6 +7632,9 @@
       <c r="P132">
         <v>1</v>
       </c>
+      <c r="Q132" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>